<commit_message>
Updated configuration file to use SGL instead of DBL for floating point values.
</commit_message>
<xml_diff>
--- a/Configuration/UDP csv Example.xlsx
+++ b/Configuration/UDP csv Example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TylerH\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\UDP-Data-Link-Custom-Device\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,9 +57,6 @@
     <t>ErrFlag12</t>
   </si>
   <si>
-    <t>Dbl</t>
-  </si>
-  <si>
     <t>FDC1BF02</t>
   </si>
   <si>
@@ -487,6 +484,9 @@
   </si>
   <si>
     <t>A brief description of the signal name which also displays in the Veristand custom device.</t>
+  </si>
+  <si>
+    <t>SGL</t>
   </si>
 </sst>
 </file>
@@ -846,7 +846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD75C62-1B41-4E95-B75B-D76A2457B859}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -870,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -898,7 +900,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -912,637 +914,637 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
         <v>71</v>
       </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
         <v>77</v>
       </c>
-      <c r="B17" t="s">
-        <v>78</v>
-      </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
         <v>83</v>
       </c>
-      <c r="B20" t="s">
-        <v>84</v>
-      </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
         <v>89</v>
       </c>
-      <c r="B23" t="s">
-        <v>90</v>
-      </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
         <v>95</v>
       </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
         <v>33</v>
       </c>
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
         <v>37</v>
       </c>
-      <c r="B33" t="s">
-        <v>38</v>
-      </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="s">
-        <v>40</v>
-      </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
         <v>41</v>
       </c>
-      <c r="B35" t="s">
-        <v>42</v>
-      </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" t="s">
         <v>43</v>
       </c>
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
       <c r="C36" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
         <v>45</v>
       </c>
-      <c r="B37" t="s">
-        <v>46</v>
-      </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
         <v>47</v>
       </c>
-      <c r="B38" t="s">
-        <v>48</v>
-      </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
         <v>59</v>
       </c>
-      <c r="B44" t="s">
-        <v>60</v>
-      </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="D49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1574,21 +1576,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started adding in the ability to type transmit channels. Still needs a lot more work to complete. Need to fix the packet reorganization in the transmit section. At a later time (before final build) the ability to reorganizae and sort receive channels/packets will be necessary.
</commit_message>
<xml_diff>
--- a/Configuration/UDP csv Example.xlsx
+++ b/Configuration/UDP csv Example.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\UDP-Data-Link-Custom-Device\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8D659F-BD55-46DD-82C4-05ED83AA3D49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{A7FED608-ED14-4349-9D93-83BF5C9257E6}"/>
   </bookViews>
@@ -42,9 +43,6 @@
     <t>ErrFlag10</t>
   </si>
   <si>
-    <t>Bool</t>
-  </si>
-  <si>
     <t>ERFLG011</t>
   </si>
   <si>
@@ -486,7 +484,10 @@
     <t>A brief description of the signal name which also displays in the Veristand custom device.</t>
   </si>
   <si>
-    <t>SGL</t>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Single</t>
   </si>
 </sst>
 </file>
@@ -846,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD75C62-1B41-4E95-B75B-D76A2457B859}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +873,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -883,668 +884,668 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" t="s">
         <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
         <v>153</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
       <c r="C7" t="s">
         <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
         <v>70</v>
       </c>
-      <c r="B14" t="s">
-        <v>71</v>
-      </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
         <v>76</v>
       </c>
-      <c r="B17" t="s">
-        <v>77</v>
-      </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="B20" t="s">
-        <v>83</v>
-      </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
         <v>94</v>
       </c>
-      <c r="B26" t="s">
-        <v>95</v>
-      </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>152</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
       <c r="C29" t="s">
         <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
       <c r="C30" t="s">
         <v>153</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
       <c r="C31" t="s">
         <v>153</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
       <c r="C32" t="s">
         <v>153</v>
       </c>
       <c r="D32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
       <c r="C33" t="s">
         <v>153</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
         <v>38</v>
       </c>
-      <c r="B34" t="s">
-        <v>39</v>
-      </c>
       <c r="C34" t="s">
         <v>153</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
         <v>40</v>
       </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
       <c r="C35" t="s">
         <v>153</v>
       </c>
       <c r="D35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
         <v>42</v>
       </c>
-      <c r="B36" t="s">
-        <v>43</v>
-      </c>
       <c r="C36" t="s">
         <v>153</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
         <v>44</v>
       </c>
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
       <c r="C37" t="s">
         <v>153</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
         <v>46</v>
       </c>
-      <c r="B38" t="s">
-        <v>47</v>
-      </c>
       <c r="C38" t="s">
         <v>153</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
         <v>153</v>
       </c>
       <c r="D39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
         <v>153</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
         <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
         <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
         <v>153</v>
       </c>
       <c r="D43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" t="s">
         <v>58</v>
       </c>
-      <c r="B44" t="s">
-        <v>59</v>
-      </c>
       <c r="C44" t="s">
         <v>153</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
         <v>153</v>
       </c>
       <c r="D45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
         <v>153</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
         <v>153</v>
       </c>
       <c r="D47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
         <v>153</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
         <v>153</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1576,21 +1577,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the binary import/export functionality. Removed some example lines from the UDP configuration files. Import of dependent channel references now works.
</commit_message>
<xml_diff>
--- a/Configuration/UDP csv Example.xlsx
+++ b/Configuration/UDP csv Example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\UDP-Data-Link-Custom-Device\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Personal Fork UDP Custom Device\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8D659F-BD55-46DD-82C4-05ED83AA3D49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D809C7BF-8720-4C44-A029-6CA7EDA5263B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{A7FED608-ED14-4349-9D93-83BF5C9257E6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="145">
   <si>
     <t>Signal Name</t>
   </si>
@@ -55,24 +55,6 @@
     <t>ErrFlag12</t>
   </si>
   <si>
-    <t>FDC1BF02</t>
-  </si>
-  <si>
-    <t>FADEC 01 BITFIELD 02</t>
-  </si>
-  <si>
-    <t>FDC1BF00</t>
-  </si>
-  <si>
-    <t>FADEC 01 BITFIELD 00</t>
-  </si>
-  <si>
-    <t>FDC1BF01</t>
-  </si>
-  <si>
-    <t>FADEC 01 BITFIELD 01</t>
-  </si>
-  <si>
     <t>28VDISC0</t>
   </si>
   <si>
@@ -335,15 +317,6 @@
   </si>
   <si>
     <t>Designates error on channel 12.</t>
-  </si>
-  <si>
-    <t>Bitfield for FADEC 01 on channel 0.</t>
-  </si>
-  <si>
-    <t>Bitfield for FADEC 01 on channel 1.</t>
-  </si>
-  <si>
-    <t>Bitfield for FADEC 01 on channel 2.</t>
   </si>
   <si>
     <t>Designates 28V power on channel 0.</t>
@@ -845,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD75C62-1B41-4E95-B75B-D76A2457B859}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -884,10 +857,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -898,10 +871,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -912,80 +885,80 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,49 +969,49 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
         <v>111</v>
@@ -1052,10 +1025,10 @@
         <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,10 +1039,10 @@
         <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1080,10 +1053,10 @@
         <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1094,10 +1067,10 @@
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D17" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1108,10 +1081,10 @@
         <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1122,10 +1095,10 @@
         <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1136,10 +1109,10 @@
         <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,10 +1123,10 @@
         <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,10 +1137,10 @@
         <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,10 +1151,10 @@
         <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,10 +1165,10 @@
         <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,52 +1179,52 @@
         <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D25" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,10 +1235,10 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,10 +1249,10 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D30" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,10 +1263,10 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,10 +1277,10 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1318,10 +1291,10 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1332,10 +1305,10 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,122 +1319,122 @@
         <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
         <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D36" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
         <v>43</v>
       </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" t="s">
         <v>52</v>
       </c>
-      <c r="B41" t="s">
-        <v>47</v>
-      </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D41" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
         <v>55</v>
       </c>
-      <c r="B42" t="s">
-        <v>53</v>
-      </c>
       <c r="C42" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D42" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
         <v>56</v>
       </c>
-      <c r="B43" t="s">
-        <v>54</v>
-      </c>
       <c r="C43" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1469,83 +1442,41 @@
         <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D45" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
         <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D46" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" t="s">
-        <v>153</v>
-      </c>
-      <c r="D47" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" t="s">
-        <v>153</v>
-      </c>
-      <c r="D48" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" t="s">
-        <v>68</v>
-      </c>
-      <c r="C49" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1577,21 +1508,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>